<commit_message>
Remake all tables for normalisation
</commit_message>
<xml_diff>
--- a/Data/services/service.xlsx
+++ b/Data/services/service.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1368" windowWidth="23040" windowHeight="9504" tabRatio="148"/>
+    <workbookView xWindow="0" yWindow="1824" windowWidth="23040" windowHeight="9504" tabRatio="148"/>
   </bookViews>
   <sheets>
     <sheet name="serv" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
-  <si>
-    <t>idServices</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>name_service</t>
   </si>
@@ -195,25 +192,7 @@
     <t>Sed mollis, eros et ultrices tempus, mauris ipsum aliquam libero,</t>
   </si>
   <si>
-    <t>Print without correction</t>
-  </si>
-  <si>
-    <t>Print with light correction</t>
-  </si>
-  <si>
-    <t>Print card with laminate</t>
-  </si>
-  <si>
-    <t>Print book with laminate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print and cuting </t>
-  </si>
-  <si>
-    <t>Print and use special paper</t>
-  </si>
-  <si>
-    <t>Special order</t>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1040,399 +1019,411 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>62</v>
+      <c r="B2" t="str">
+        <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65,95)), CHAR(RANDBETWEEN(65,95)), RANDBETWEEN(1,2000), RANDBETWEEN(65,95), CHAR(RANDBETWEEN(65,95)))</f>
+        <v>JA117277O</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(350, 1000)</f>
-        <v>684</v>
+        <v>395</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">CONCATENATE("#", RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), RANDBETWEEN(1,28))</f>
-        <v>#201219</v>
+        <v>#200353</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F51" ca="1" si="0">RANDBETWEEN(1,50)</f>
-        <v>34</v>
+        <f ca="1">RANDBETWEEN(1,49)</f>
+        <v>25</v>
       </c>
       <c r="G2" s="2">
         <f ca="1">DATE(RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), DAY(RANDBETWEEN(1,28)))</f>
-        <v>38172</v>
+        <v>43023</v>
       </c>
       <c r="H2">
         <f ca="1">RANDBETWEEN(1,50)</f>
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>58</v>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B51" ca="1" si="0">CONCATENATE(CHAR(RANDBETWEEN(65,95)), CHAR(RANDBETWEEN(65,95)), RANDBETWEEN(1,2000), RANDBETWEEN(65,95), CHAR(RANDBETWEEN(65,95)))</f>
+        <v>RI168181Z</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D51" ca="1" si="1">RANDBETWEEN(350, 1000)</f>
-        <v>845</v>
+        <v>380</v>
       </c>
       <c r="E3" s="2" t="str">
         <f ca="1">CONCATENATE("#", RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), RANDBETWEEN(1,28))</f>
-        <v>#200078</v>
+        <v>#2008112</v>
       </c>
       <c r="F3">
-        <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <f t="shared" ref="F3:F51" ca="1" si="2">RANDBETWEEN(1,49)</f>
+        <v>33</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G51" ca="1" si="2">DATE(RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), DAY(RANDBETWEEN(1,28)))</f>
-        <v>39180</v>
+        <f t="shared" ref="G3:G51" ca="1" si="3">DATE(RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), DAY(RANDBETWEEN(1,28)))</f>
+        <v>39318</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H51" ca="1" si="3">RANDBETWEEN(1,50)</f>
-        <v>23</v>
+        <f t="shared" ref="H3:H51" ca="1" si="4">RANDBETWEEN(1,50)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>58</v>
+      <c r="B4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BY30993A</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>551</v>
+        <v>425</v>
       </c>
       <c r="E4" s="2" t="str">
-        <f t="shared" ref="E4:E51" ca="1" si="4">CONCATENATE("#", RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), RANDBETWEEN(1,28))</f>
-        <v>#20201211</v>
+        <f t="shared" ref="E4:E51" ca="1" si="5">CONCATENATE("#", RANDBETWEEN(2000,2020), RANDBETWEEN(1,12), RANDBETWEEN(1,28))</f>
+        <v>#2003125</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>41717</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>41344</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>59</v>
+      <c r="B5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>JT80683W</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>411</v>
+        <v>375</v>
       </c>
       <c r="E5" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2005625</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#20081115</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>41</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38005</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>41768</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="3"/>
-        <v>49</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>64</v>
+      <c r="B6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>HL160074X</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>477</v>
+        <v>408</v>
       </c>
       <c r="E6" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2014619</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2012219</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>25</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42518</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>42172</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>59</v>
+      <c r="B7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>IC45994_</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>568</v>
+        <v>525</v>
       </c>
       <c r="E7" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2013117</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#201426</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42963</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>37869</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>58</v>
+      <c r="B8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>PA15072P</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>676</v>
+        <v>443</v>
       </c>
       <c r="E8" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#200273</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2012119</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>48</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38385</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>36996</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>62</v>
+      <c r="B9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>QO21985Y</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>583</v>
+        <v>903</v>
       </c>
       <c r="E9" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2012219</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2016720</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42561</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>38203</v>
       </c>
       <c r="H9">
-        <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>58</v>
+      <c r="B10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BI85584N</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>498</v>
+        <v>554</v>
       </c>
       <c r="E10" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#200988</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#200454</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>38</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>39979</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>39399</v>
       </c>
       <c r="H10">
-        <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>59</v>
+      <c r="B11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>SQ44368B</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>442</v>
+        <v>487</v>
       </c>
       <c r="E11" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#201364</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2005113</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42261</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>44008</v>
       </c>
       <c r="H11">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>64</v>
+      <c r="B12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>RD62670C</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>571</v>
+        <v>550</v>
       </c>
       <c r="E12" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#200938</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2000823</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>37756</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>37702</v>
       </c>
       <c r="H12">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>63</v>
+      <c r="B13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>GG188892W</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>446</v>
+        <v>862</v>
       </c>
       <c r="E13" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2014910</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2013224</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38024</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>38185</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>31</v>
       </c>
     </row>
@@ -1440,712 +1431,735 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>58</v>
+      <c r="B14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>DP192066J</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>688</v>
+        <v>890</v>
       </c>
       <c r="E14" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#202089</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#200378</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38180</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43195</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>58</v>
+      <c r="B15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>EP70583C</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>841</v>
+        <v>932</v>
       </c>
       <c r="E15" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2009109</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2003912</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38189</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>37093</v>
       </c>
       <c r="H15">
-        <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>59</v>
+      <c r="B16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>]G51970A</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>559</v>
+        <v>788</v>
       </c>
       <c r="E16" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#20091024</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2005311</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>39047</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>41300</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>58</v>
+      <c r="B17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>IL169874N</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>659</v>
+        <v>680</v>
       </c>
       <c r="E17" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#20161012</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2019813</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>37905</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>40029</v>
       </c>
       <c r="H17">
-        <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>62</v>
+      <c r="B18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>ON59575R</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>843</v>
+        <v>978</v>
       </c>
       <c r="E18" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2012127</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2009422</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42965</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43350</v>
       </c>
       <c r="H18">
-        <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>58</v>
+      <c r="B19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>RQ184774X</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>398</v>
+        <v>956</v>
       </c>
       <c r="E19" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2016523</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2020327</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>39931</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>39408</v>
       </c>
       <c r="H19">
-        <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>59</v>
+      <c r="B20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>^Y181671L</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>938</v>
+        <v>851</v>
       </c>
       <c r="E20" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2020120</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2006715</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>35</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>43725</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43774</v>
       </c>
       <c r="H20">
-        <f t="shared" ca="1" si="3"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>63</v>
+      <c r="B21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NM119169W</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>900</v>
+        <v>401</v>
       </c>
       <c r="E21" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2007814</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2008414</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>33</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40884</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>40016</v>
       </c>
       <c r="H21">
-        <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>62</v>
+      <c r="B22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>HI79669W</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>927</v>
+        <v>525</v>
       </c>
       <c r="E22" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2004910</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2010719</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38548</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>39176</v>
       </c>
       <c r="H22">
-        <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>58</v>
+      <c r="B23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>U_84887_</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>361</v>
+        <v>724</v>
       </c>
       <c r="E23" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2019312</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2000716</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38642</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43175</v>
       </c>
       <c r="H23">
-        <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>60</v>
+      <c r="B24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>EN144489A</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>677</v>
+        <v>484</v>
       </c>
       <c r="E24" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2011118</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#20071223</v>
       </c>
       <c r="F24">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>43832</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>42806</v>
       </c>
       <c r="H24">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>59</v>
+      <c r="B25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>YW153785P</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>423</v>
+        <v>953</v>
       </c>
       <c r="E25" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2001923</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2016722</v>
       </c>
       <c r="F25">
-        <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40608</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>38596</v>
       </c>
       <c r="H25">
-        <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>63</v>
+      <c r="B26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LO87793_</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>446</v>
+        <v>383</v>
       </c>
       <c r="E26" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2019108</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2007511</v>
       </c>
       <c r="F26">
-        <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>43</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40398</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43043</v>
       </c>
       <c r="H26">
-        <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>61</v>
+      <c r="B27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>QQ183681C</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="E27" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#20131110</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2017825</v>
       </c>
       <c r="F27">
-        <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>32</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38687</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>38704</v>
       </c>
       <c r="H27">
-        <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>62</v>
+      <c r="B28" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>_I96993A</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>563</v>
+        <v>666</v>
       </c>
       <c r="E28" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2009114</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2010722</v>
       </c>
       <c r="F28">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40012</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>40668</v>
       </c>
       <c r="H28">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>60</v>
+      <c r="B29" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>CS102378W</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>999</v>
+        <v>982</v>
       </c>
       <c r="E29" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2020915</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2000711</v>
       </c>
       <c r="F29">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40780</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43628</v>
       </c>
       <c r="H29">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>61</v>
+      <c r="B30" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>V\21787_</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>921</v>
+        <v>728</v>
       </c>
       <c r="E30" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#201597</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2014210</v>
       </c>
       <c r="F30">
-        <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>44106</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>41945</v>
       </c>
       <c r="H30">
-        <f t="shared" ca="1" si="3"/>
-        <v>21</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>64</v>
+      <c r="B31" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>R^49883T</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="1"/>
-        <v>530</v>
+        <v>404</v>
       </c>
       <c r="E31" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2020627</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2007921</v>
       </c>
       <c r="F31">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>48</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>39663</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>42868</v>
       </c>
       <c r="H31">
-        <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>63</v>
+      <c r="B32" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>T^135167_</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="1"/>
-        <v>910</v>
+        <v>778</v>
       </c>
       <c r="E32" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2001113</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2017414</v>
       </c>
       <c r="F32">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>48</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42771</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>42250</v>
       </c>
       <c r="H32">
-        <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>61</v>
+      <c r="B33" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>^K93391F</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="1"/>
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E33" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#20091114</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2020228</v>
       </c>
       <c r="F33">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>39571</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>39718</v>
       </c>
       <c r="H33">
-        <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>58</v>
+      <c r="B34" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>]]95475K</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
-        <v>889</v>
+        <v>515</v>
       </c>
       <c r="E34" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2001621</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#200637</v>
       </c>
       <c r="F34">
-        <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>37605</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>37997</v>
       </c>
       <c r="H34">
-        <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>62</v>
+      <c r="B35" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>EF180588E</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="1"/>
-        <v>735</v>
+        <v>851</v>
       </c>
       <c r="E35" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2008913</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2020914</v>
       </c>
       <c r="F35">
-        <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38549</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>36569</v>
       </c>
       <c r="H35">
-        <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>58</v>
+      <c r="B36" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>XZ56790\</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="1"/>
-        <v>585</v>
+        <v>529</v>
       </c>
       <c r="E36" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2013115</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#201097</v>
       </c>
       <c r="F36">
-        <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42526</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>41744</v>
       </c>
       <c r="H36">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="4"/>
         <v>41</v>
       </c>
     </row>
@@ -2153,465 +2167,480 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>63</v>
+      <c r="B37" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>XZ132395G</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="1"/>
-        <v>885</v>
+        <v>375</v>
       </c>
       <c r="E37" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2017718</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#202032</v>
       </c>
       <c r="F37">
-        <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40059</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43089</v>
       </c>
       <c r="H37">
-        <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>61</v>
+      <c r="B38" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>TY19594S</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="1"/>
-        <v>369</v>
+        <v>716</v>
       </c>
       <c r="E38" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2016922</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2019112</v>
       </c>
       <c r="F38">
-        <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>36</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>41062</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>37697</v>
       </c>
       <c r="H38">
-        <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>58</v>
+      <c r="B39" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>[H170578N</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="1"/>
-        <v>908</v>
+        <v>637</v>
       </c>
       <c r="E39" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#20001113</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#20161211</v>
       </c>
       <c r="F39">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>36</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38099</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>38463</v>
       </c>
       <c r="H39">
-        <f t="shared" ca="1" si="3"/>
-        <v>44</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>64</v>
+      <c r="B40" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>S]30567_</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="1"/>
-        <v>882</v>
+        <v>798</v>
       </c>
       <c r="E40" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2017114</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2000213</v>
       </c>
       <c r="F40">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
       </c>
       <c r="G40" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>41655</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43954</v>
       </c>
       <c r="H40">
-        <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
-        <v>59</v>
+      <c r="B41" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>JE88182A</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="1"/>
-        <v>788</v>
+        <v>687</v>
       </c>
       <c r="E41" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#20011214</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2015418</v>
       </c>
       <c r="F41">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>36927</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ca="1" si="4"/>
         <v>2</v>
-      </c>
-      <c r="G41" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40756</v>
-      </c>
-      <c r="H41">
-        <f t="shared" ca="1" si="3"/>
-        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
-        <v>58</v>
+      <c r="B42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>TZ77781H</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="1"/>
-        <v>479</v>
+        <v>537</v>
       </c>
       <c r="E42" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2013418</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2008320</v>
       </c>
       <c r="F42">
-        <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>21</v>
       </c>
       <c r="G42" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>39160</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>42753</v>
       </c>
       <c r="H42">
-        <f t="shared" ca="1" si="3"/>
-        <v>40</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
-        <v>61</v>
+      <c r="B43" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>RC39089_</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="1"/>
-        <v>566</v>
+        <v>654</v>
       </c>
       <c r="E43" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2018315</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2009210</v>
       </c>
       <c r="F43">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>43</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>39335</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>37288</v>
       </c>
       <c r="H43">
-        <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
-        <v>58</v>
+      <c r="B44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>AT56094_</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="1"/>
-        <v>906</v>
+        <v>388</v>
       </c>
       <c r="E44" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2001621</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2017418</v>
       </c>
       <c r="F44">
-        <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45</v>
       </c>
       <c r="G44" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>40601</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43755</v>
       </c>
       <c r="H44">
-        <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>58</v>
+      <c r="B45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>B]186667F</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="1"/>
-        <v>810</v>
+        <v>823</v>
       </c>
       <c r="E45" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2010726</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2004910</v>
       </c>
       <c r="F45">
-        <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
       </c>
       <c r="G45" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>38330</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>43244</v>
       </c>
       <c r="H45">
-        <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>59</v>
+      <c r="B46" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>LV136183H</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="1"/>
-        <v>523</v>
+        <v>640</v>
       </c>
       <c r="E46" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#200917</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2007103</v>
       </c>
       <c r="F46">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>47</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>41034</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>39479</v>
       </c>
       <c r="H46">
-        <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
-        <v>60</v>
+      <c r="B47" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>WV106466Q</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="1"/>
-        <v>693</v>
+        <v>867</v>
       </c>
       <c r="E47" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2019627</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2001314</v>
       </c>
       <c r="F47">
-        <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
       </c>
       <c r="G47" s="2">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>36666</v>
       </c>
       <c r="H47">
-        <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
-        <v>63</v>
+      <c r="B48" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>WL76475S</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="1"/>
-        <v>922</v>
+        <v>578</v>
       </c>
       <c r="E48" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2015524</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#20081110</v>
       </c>
       <c r="F48">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
       </c>
       <c r="G48" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>41226</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>38835</v>
       </c>
       <c r="H48">
-        <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
-        <v>58</v>
+      <c r="B49" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>KR172365B</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="1"/>
-        <v>619</v>
+        <v>629</v>
       </c>
       <c r="E49" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#20191019</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#201011</v>
       </c>
       <c r="F49">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
       </c>
       <c r="G49" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>37971</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>37472</v>
       </c>
       <c r="H49">
-        <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
-        <v>60</v>
+      <c r="B50" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>SM121968S</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="1"/>
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="E50" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#200652</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2003112</v>
       </c>
       <c r="F50">
-        <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>44070</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>40140</v>
       </c>
       <c r="H50">
-        <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
-        <v>58</v>
+      <c r="B51" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>UR170675P</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="1"/>
-        <v>466</v>
+        <v>979</v>
       </c>
       <c r="E51" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>#2017420</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>#2003714</v>
       </c>
       <c r="F51">
-        <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>42994</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>44160</v>
       </c>
       <c r="H51">
-        <f t="shared" ca="1" si="3"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>